<commit_message>
Shared ESS model update.
</commit_message>
<xml_diff>
--- a/data/CS1_2/Market Data/CS1_market_data_2020.xlsx
+++ b/data/CS1_2/Market Data/CS1_market_data_2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\shared-resources-planning-v3\data\HR1\Market Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\shared-resources-planning-v3\data\CS1_2\Market Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{806A7DB6-DD20-43BF-BEB7-AB2DCFB01203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0852FE-AAE0-45CD-8C5B-97B961FBADC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,10 @@
     <sheet name="Csr, Winter" sheetId="3" r:id="rId3"/>
     <sheet name="Ctr_up, Winter" sheetId="4" r:id="rId4"/>
     <sheet name="Ctr_down, Winter" sheetId="5" r:id="rId5"/>
-    <sheet name="Cp, Summer" sheetId="6" r:id="rId6"/>
-    <sheet name="Csr, Summer" sheetId="7" r:id="rId7"/>
-    <sheet name="Ctr_up, Summer" sheetId="8" r:id="rId8"/>
-    <sheet name="Ctr_down, Summer" sheetId="9" r:id="rId9"/>
+    <sheet name="Cp, Summer" sheetId="10" r:id="rId6"/>
+    <sheet name="Csr, Summer" sheetId="11" r:id="rId7"/>
+    <sheet name="Ctr_up, Summer" sheetId="12" r:id="rId8"/>
+    <sheet name="Ctr_down, Summer" sheetId="13" r:id="rId9"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId10"/>
@@ -131,33 +131,31 @@
       <sheetName val="Secondary Reserve, Winter"/>
       <sheetName val="Tertiary Reserve Up, Winter"/>
       <sheetName val="Tertiary Reserve Down, Winter"/>
-      <sheetName val="Flexibility, Winter"/>
       <sheetName val="Energy, Summer"/>
       <sheetName val="Secondary Reserve, Summer"/>
       <sheetName val="Tertiary Reserve Up, Summer"/>
       <sheetName val="Tertiary Reserve Down, Summer"/>
-      <sheetName val="Flexibility, Summer"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>0</v>
+            <v>0.05</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>5.0000000000000001E-3</v>
+            <v>0.05</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>5.0000000000000001E-3</v>
+            <v>0.05</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5">
-            <v>5.0000000000000001E-3</v>
+            <v>0.05</v>
           </cell>
         </row>
       </sheetData>
@@ -1088,7 +1086,6 @@
           <cell r="L4">
             <v>44</v>
           </cell>
-          <cell r="M4"/>
           <cell r="N4">
             <v>46</v>
           </cell>
@@ -1647,8 +1644,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6">
+      <sheetData sheetId="5">
         <row r="2">
           <cell r="B2">
             <v>35.549999999999997</v>
@@ -2017,756 +2013,756 @@
           </cell>
           <cell r="Y6">
             <v>36</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6">
+        <row r="2">
+          <cell r="B2">
+            <v>6.52</v>
+          </cell>
+          <cell r="C2">
+            <v>10.56</v>
+          </cell>
+          <cell r="D2">
+            <v>5.92</v>
+          </cell>
+          <cell r="E2">
+            <v>6.15</v>
+          </cell>
+          <cell r="F2">
+            <v>6.79</v>
+          </cell>
+          <cell r="G2">
+            <v>6.65</v>
+          </cell>
+          <cell r="H2">
+            <v>10</v>
+          </cell>
+          <cell r="I2">
+            <v>10.19</v>
+          </cell>
+          <cell r="J2">
+            <v>9.76</v>
+          </cell>
+          <cell r="K2">
+            <v>8.0500000000000007</v>
+          </cell>
+          <cell r="L2">
+            <v>8.66</v>
+          </cell>
+          <cell r="M2">
+            <v>10</v>
+          </cell>
+          <cell r="N2">
+            <v>7.8</v>
+          </cell>
+          <cell r="O2">
+            <v>5.82</v>
+          </cell>
+          <cell r="P2">
+            <v>6.56</v>
+          </cell>
+          <cell r="Q2">
+            <v>8.0399999999999991</v>
+          </cell>
+          <cell r="R2">
+            <v>7.63</v>
+          </cell>
+          <cell r="S2">
+            <v>8.42</v>
+          </cell>
+          <cell r="T2">
+            <v>4.66</v>
+          </cell>
+          <cell r="U2">
+            <v>4.32</v>
+          </cell>
+          <cell r="V2">
+            <v>2.81</v>
+          </cell>
+          <cell r="W2">
+            <v>2.81</v>
+          </cell>
+          <cell r="X2">
+            <v>3.33</v>
+          </cell>
+          <cell r="Y2">
+            <v>8.9700000000000006</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3">
+            <v>11.27</v>
+          </cell>
+          <cell r="C3">
+            <v>12.24</v>
+          </cell>
+          <cell r="D3">
+            <v>8.3699999999999992</v>
+          </cell>
+          <cell r="E3">
+            <v>8.5399999999999991</v>
+          </cell>
+          <cell r="F3">
+            <v>8.84</v>
+          </cell>
+          <cell r="G3">
+            <v>8.93</v>
+          </cell>
+          <cell r="H3">
+            <v>17.93</v>
+          </cell>
+          <cell r="I3">
+            <v>15.6</v>
+          </cell>
+          <cell r="J3">
+            <v>9.8800000000000008</v>
+          </cell>
+          <cell r="K3">
+            <v>9.6300000000000008</v>
+          </cell>
+          <cell r="L3">
+            <v>7.71</v>
+          </cell>
+          <cell r="M3">
+            <v>7.97</v>
+          </cell>
+          <cell r="N3">
+            <v>9.08</v>
+          </cell>
+          <cell r="O3">
+            <v>7.13</v>
+          </cell>
+          <cell r="P3">
+            <v>7.4</v>
+          </cell>
+          <cell r="Q3">
+            <v>7.84</v>
+          </cell>
+          <cell r="R3">
+            <v>7.6</v>
+          </cell>
+          <cell r="S3">
+            <v>5.7</v>
+          </cell>
+          <cell r="T3">
+            <v>4.8499999999999996</v>
+          </cell>
+          <cell r="U3">
+            <v>4.2300000000000004</v>
+          </cell>
+          <cell r="V3">
+            <v>2.38</v>
+          </cell>
+          <cell r="W3">
+            <v>2.8</v>
+          </cell>
+          <cell r="X3">
+            <v>2.09</v>
+          </cell>
+          <cell r="Y3">
+            <v>12.33</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4">
+            <v>5.88</v>
+          </cell>
+          <cell r="C4">
+            <v>8.98</v>
+          </cell>
+          <cell r="D4">
+            <v>7.64</v>
+          </cell>
+          <cell r="E4">
+            <v>7.72</v>
+          </cell>
+          <cell r="F4">
+            <v>7.64</v>
+          </cell>
+          <cell r="G4">
+            <v>7.72</v>
+          </cell>
+          <cell r="H4">
+            <v>8.23</v>
+          </cell>
+          <cell r="I4">
+            <v>7.19</v>
+          </cell>
+          <cell r="J4">
+            <v>6.72</v>
+          </cell>
+          <cell r="K4">
+            <v>6.56</v>
+          </cell>
+          <cell r="L4">
+            <v>5.75</v>
+          </cell>
+          <cell r="M4">
+            <v>4.9400000000000004</v>
+          </cell>
+          <cell r="N4">
+            <v>4.6100000000000003</v>
+          </cell>
+          <cell r="O4">
+            <v>4.6100000000000003</v>
+          </cell>
+          <cell r="P4">
+            <v>6.11</v>
+          </cell>
+          <cell r="Q4">
+            <v>4.6100000000000003</v>
+          </cell>
+          <cell r="R4">
+            <v>4.6100000000000003</v>
+          </cell>
+          <cell r="S4">
+            <v>4.66</v>
+          </cell>
+          <cell r="T4">
+            <v>5.58</v>
+          </cell>
+          <cell r="U4">
+            <v>5.56</v>
+          </cell>
+          <cell r="V4">
+            <v>5.09</v>
+          </cell>
+          <cell r="W4">
+            <v>4.33</v>
+          </cell>
+          <cell r="X4">
+            <v>4.62</v>
+          </cell>
+          <cell r="Y4">
+            <v>6.95</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5">
+            <v>11.09</v>
+          </cell>
+          <cell r="C5">
+            <v>18.989999999999998</v>
+          </cell>
+          <cell r="D5">
+            <v>10.62</v>
+          </cell>
+          <cell r="E5">
+            <v>10.62</v>
+          </cell>
+          <cell r="F5">
+            <v>10.62</v>
+          </cell>
+          <cell r="G5">
+            <v>10.62</v>
+          </cell>
+          <cell r="H5">
+            <v>10.42</v>
+          </cell>
+          <cell r="I5">
+            <v>6.72</v>
+          </cell>
+          <cell r="J5">
+            <v>6.96</v>
+          </cell>
+          <cell r="K5">
+            <v>7.46</v>
+          </cell>
+          <cell r="L5">
+            <v>10.48</v>
+          </cell>
+          <cell r="M5">
+            <v>9.4</v>
+          </cell>
+          <cell r="N5">
+            <v>8.4600000000000009</v>
+          </cell>
+          <cell r="O5">
+            <v>8.6300000000000008</v>
+          </cell>
+          <cell r="P5">
+            <v>8.4600000000000009</v>
+          </cell>
+          <cell r="Q5">
+            <v>10.89</v>
+          </cell>
+          <cell r="R5">
+            <v>9.8699999999999992</v>
+          </cell>
+          <cell r="S5">
+            <v>8.06</v>
+          </cell>
+          <cell r="T5">
+            <v>8.06</v>
+          </cell>
+          <cell r="U5">
+            <v>8.75</v>
+          </cell>
+          <cell r="V5">
+            <v>6.17</v>
+          </cell>
+          <cell r="W5">
+            <v>6.6</v>
+          </cell>
+          <cell r="X5">
+            <v>5.72</v>
+          </cell>
+          <cell r="Y5">
+            <v>10.26</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6">
+            <v>7.58</v>
+          </cell>
+          <cell r="C6">
+            <v>9.4499999999999993</v>
+          </cell>
+          <cell r="D6">
+            <v>6.33</v>
+          </cell>
+          <cell r="E6">
+            <v>6.8</v>
+          </cell>
+          <cell r="F6">
+            <v>6.8</v>
+          </cell>
+          <cell r="G6">
+            <v>6.25</v>
+          </cell>
+          <cell r="H6">
+            <v>7.77</v>
+          </cell>
+          <cell r="I6">
+            <v>9.4499999999999993</v>
+          </cell>
+          <cell r="J6">
+            <v>9.2200000000000006</v>
+          </cell>
+          <cell r="K6">
+            <v>8.6199999999999992</v>
+          </cell>
+          <cell r="L6">
+            <v>7.09</v>
+          </cell>
+          <cell r="M6">
+            <v>6.43</v>
+          </cell>
+          <cell r="N6">
+            <v>5.85</v>
+          </cell>
+          <cell r="O6">
+            <v>6.44</v>
+          </cell>
+          <cell r="P6">
+            <v>6.79</v>
+          </cell>
+          <cell r="Q6">
+            <v>8.14</v>
+          </cell>
+          <cell r="R6">
+            <v>8.51</v>
+          </cell>
+          <cell r="S6">
+            <v>9.17</v>
+          </cell>
+          <cell r="T6">
+            <v>8.7899999999999991</v>
+          </cell>
+          <cell r="U6">
+            <v>7.6</v>
+          </cell>
+          <cell r="V6">
+            <v>6.29</v>
+          </cell>
+          <cell r="W6">
+            <v>6.62</v>
+          </cell>
+          <cell r="X6">
+            <v>6.53</v>
+          </cell>
+          <cell r="Y6">
+            <v>7.99</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="7">
         <row r="2">
           <cell r="B2">
-            <v>6.52</v>
+            <v>36.4</v>
           </cell>
           <cell r="C2">
-            <v>10.56</v>
+            <v>36.4</v>
           </cell>
           <cell r="D2">
-            <v>5.92</v>
+            <v>35.69</v>
           </cell>
           <cell r="E2">
-            <v>6.15</v>
+            <v>35.69</v>
           </cell>
           <cell r="F2">
-            <v>6.79</v>
+            <v>35.69</v>
           </cell>
           <cell r="G2">
-            <v>6.65</v>
+            <v>35.69</v>
           </cell>
           <cell r="H2">
-            <v>10</v>
+            <v>35.69</v>
           </cell>
           <cell r="I2">
-            <v>10.19</v>
+            <v>47.22</v>
           </cell>
           <cell r="J2">
-            <v>9.76</v>
+            <v>36.4</v>
           </cell>
           <cell r="K2">
-            <v>8.0500000000000007</v>
+            <v>36.4</v>
           </cell>
           <cell r="L2">
-            <v>8.66</v>
+            <v>47.22</v>
           </cell>
           <cell r="M2">
-            <v>10</v>
+            <v>47.22</v>
           </cell>
           <cell r="N2">
-            <v>7.8</v>
+            <v>42</v>
           </cell>
           <cell r="O2">
-            <v>5.82</v>
+            <v>38</v>
           </cell>
           <cell r="P2">
-            <v>6.56</v>
+            <v>38</v>
           </cell>
           <cell r="Q2">
-            <v>8.0399999999999991</v>
+            <v>47.22</v>
           </cell>
           <cell r="R2">
-            <v>7.63</v>
+            <v>47.22</v>
           </cell>
           <cell r="S2">
-            <v>8.42</v>
+            <v>47.22</v>
           </cell>
           <cell r="T2">
-            <v>4.66</v>
+            <v>47.22</v>
           </cell>
           <cell r="U2">
-            <v>4.32</v>
+            <v>47.22</v>
           </cell>
           <cell r="V2">
-            <v>2.81</v>
+            <v>47.22</v>
           </cell>
           <cell r="W2">
-            <v>2.81</v>
+            <v>47.22</v>
           </cell>
           <cell r="X2">
-            <v>3.33</v>
+            <v>47.22</v>
           </cell>
           <cell r="Y2">
-            <v>8.9700000000000006</v>
+            <v>47.22</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>11.27</v>
+            <v>47.22</v>
           </cell>
           <cell r="C3">
-            <v>12.24</v>
+            <v>47.22</v>
           </cell>
           <cell r="D3">
-            <v>8.3699999999999992</v>
+            <v>47.22</v>
           </cell>
           <cell r="E3">
-            <v>8.5399999999999991</v>
+            <v>36</v>
           </cell>
           <cell r="F3">
-            <v>8.84</v>
+            <v>35.69</v>
           </cell>
           <cell r="G3">
-            <v>8.93</v>
+            <v>35.69</v>
           </cell>
           <cell r="H3">
-            <v>17.93</v>
+            <v>35.69</v>
           </cell>
           <cell r="I3">
-            <v>15.6</v>
+            <v>47.22</v>
           </cell>
           <cell r="J3">
-            <v>9.8800000000000008</v>
+            <v>47.22</v>
           </cell>
           <cell r="K3">
-            <v>9.6300000000000008</v>
+            <v>47.22</v>
           </cell>
           <cell r="L3">
-            <v>7.71</v>
+            <v>47.22</v>
           </cell>
           <cell r="M3">
-            <v>7.97</v>
+            <v>47.22</v>
           </cell>
           <cell r="N3">
-            <v>9.08</v>
+            <v>47.22</v>
           </cell>
           <cell r="O3">
-            <v>7.13</v>
+            <v>47.22</v>
           </cell>
           <cell r="P3">
-            <v>7.4</v>
+            <v>47.22</v>
           </cell>
           <cell r="Q3">
-            <v>7.84</v>
+            <v>47.22</v>
           </cell>
           <cell r="R3">
-            <v>7.6</v>
+            <v>47.22</v>
           </cell>
           <cell r="S3">
-            <v>5.7</v>
+            <v>47.22</v>
           </cell>
           <cell r="T3">
-            <v>4.8499999999999996</v>
+            <v>47.22</v>
           </cell>
           <cell r="U3">
-            <v>4.2300000000000004</v>
+            <v>47.22</v>
           </cell>
           <cell r="V3">
-            <v>2.38</v>
+            <v>47.22</v>
           </cell>
           <cell r="W3">
-            <v>2.8</v>
+            <v>47.22</v>
           </cell>
           <cell r="X3">
-            <v>2.09</v>
+            <v>36</v>
           </cell>
           <cell r="Y3">
-            <v>12.33</v>
+            <v>47.22</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>5.88</v>
+            <v>47.22</v>
           </cell>
           <cell r="C4">
-            <v>8.98</v>
+            <v>37.4</v>
           </cell>
           <cell r="D4">
-            <v>7.64</v>
+            <v>69.040000000000006</v>
           </cell>
           <cell r="E4">
-            <v>7.72</v>
+            <v>37.4</v>
           </cell>
           <cell r="F4">
-            <v>7.64</v>
+            <v>35.69</v>
           </cell>
           <cell r="G4">
-            <v>7.72</v>
+            <v>37.4</v>
           </cell>
           <cell r="H4">
-            <v>8.23</v>
+            <v>37.4</v>
           </cell>
           <cell r="I4">
-            <v>7.19</v>
+            <v>37.4</v>
           </cell>
           <cell r="J4">
-            <v>6.72</v>
+            <v>37.4</v>
           </cell>
           <cell r="K4">
-            <v>6.56</v>
+            <v>38</v>
           </cell>
           <cell r="L4">
-            <v>5.75</v>
+            <v>38</v>
           </cell>
           <cell r="M4">
-            <v>4.9400000000000004</v>
+            <v>47.22</v>
           </cell>
           <cell r="N4">
-            <v>4.6100000000000003</v>
+            <v>47.22</v>
           </cell>
           <cell r="O4">
-            <v>4.6100000000000003</v>
+            <v>47.22</v>
           </cell>
           <cell r="P4">
-            <v>6.11</v>
+            <v>47.22</v>
           </cell>
           <cell r="Q4">
-            <v>4.6100000000000003</v>
+            <v>47.22</v>
           </cell>
           <cell r="R4">
-            <v>4.6100000000000003</v>
+            <v>47.22</v>
           </cell>
           <cell r="S4">
-            <v>4.66</v>
+            <v>47.22</v>
           </cell>
           <cell r="T4">
-            <v>5.58</v>
+            <v>47.22</v>
           </cell>
           <cell r="U4">
-            <v>5.56</v>
+            <v>47.22</v>
           </cell>
           <cell r="V4">
-            <v>5.09</v>
+            <v>47.22</v>
           </cell>
           <cell r="W4">
-            <v>4.33</v>
+            <v>95</v>
           </cell>
           <cell r="X4">
-            <v>4.62</v>
+            <v>47.22</v>
           </cell>
           <cell r="Y4">
-            <v>6.95</v>
+            <v>47.22</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5">
-            <v>11.09</v>
+            <v>37</v>
           </cell>
           <cell r="C5">
-            <v>18.989999999999998</v>
+            <v>35.69</v>
           </cell>
           <cell r="D5">
-            <v>10.62</v>
+            <v>35.69</v>
           </cell>
           <cell r="E5">
-            <v>10.62</v>
+            <v>35.69</v>
           </cell>
           <cell r="F5">
-            <v>10.62</v>
+            <v>35.69</v>
           </cell>
           <cell r="G5">
-            <v>10.62</v>
+            <v>35.69</v>
           </cell>
           <cell r="H5">
-            <v>10.42</v>
+            <v>47.22</v>
           </cell>
           <cell r="I5">
-            <v>6.72</v>
+            <v>47.22</v>
           </cell>
           <cell r="J5">
-            <v>6.96</v>
+            <v>47.22</v>
           </cell>
           <cell r="K5">
-            <v>7.46</v>
+            <v>47.22</v>
           </cell>
           <cell r="L5">
-            <v>10.48</v>
+            <v>36</v>
           </cell>
           <cell r="M5">
-            <v>9.4</v>
+            <v>38.4</v>
           </cell>
           <cell r="N5">
-            <v>8.4600000000000009</v>
+            <v>47.22</v>
           </cell>
           <cell r="O5">
-            <v>8.6300000000000008</v>
+            <v>47.22</v>
           </cell>
           <cell r="P5">
-            <v>8.4600000000000009</v>
+            <v>47.22</v>
           </cell>
           <cell r="Q5">
-            <v>10.89</v>
+            <v>47.22</v>
           </cell>
           <cell r="R5">
-            <v>9.8699999999999992</v>
+            <v>47.22</v>
           </cell>
           <cell r="S5">
-            <v>8.06</v>
+            <v>47.22</v>
           </cell>
           <cell r="T5">
-            <v>8.06</v>
+            <v>47.22</v>
           </cell>
           <cell r="U5">
-            <v>8.75</v>
+            <v>47.22</v>
           </cell>
           <cell r="V5">
-            <v>6.17</v>
+            <v>47.12</v>
           </cell>
           <cell r="W5">
-            <v>6.6</v>
+            <v>47.22</v>
           </cell>
           <cell r="X5">
-            <v>5.72</v>
+            <v>47.22</v>
           </cell>
           <cell r="Y5">
-            <v>10.26</v>
+            <v>47.043333333333329</v>
           </cell>
         </row>
         <row r="6">
           <cell r="B6">
-            <v>7.58</v>
+            <v>46.66</v>
           </cell>
           <cell r="C6">
-            <v>9.4499999999999993</v>
+            <v>46.69</v>
           </cell>
           <cell r="D6">
-            <v>6.33</v>
+            <v>37.4</v>
           </cell>
           <cell r="E6">
-            <v>6.8</v>
+            <v>37.4</v>
           </cell>
           <cell r="F6">
-            <v>6.8</v>
+            <v>37.4</v>
           </cell>
           <cell r="G6">
-            <v>6.25</v>
+            <v>37.4</v>
           </cell>
           <cell r="H6">
-            <v>7.77</v>
+            <v>47.22</v>
           </cell>
           <cell r="I6">
-            <v>9.4499999999999993</v>
+            <v>64.64</v>
           </cell>
           <cell r="J6">
-            <v>9.2200000000000006</v>
+            <v>37.4</v>
           </cell>
           <cell r="K6">
-            <v>8.6199999999999992</v>
+            <v>37.4</v>
           </cell>
           <cell r="L6">
-            <v>7.09</v>
+            <v>36</v>
           </cell>
           <cell r="M6">
-            <v>6.43</v>
+            <v>37.4</v>
           </cell>
           <cell r="N6">
-            <v>5.85</v>
+            <v>46.69</v>
           </cell>
           <cell r="O6">
-            <v>6.44</v>
+            <v>46.69</v>
           </cell>
           <cell r="P6">
-            <v>6.79</v>
+            <v>46.69</v>
           </cell>
           <cell r="Q6">
-            <v>8.14</v>
+            <v>46.69</v>
           </cell>
           <cell r="R6">
-            <v>8.51</v>
+            <v>46.69</v>
           </cell>
           <cell r="S6">
-            <v>9.17</v>
+            <v>46.69</v>
           </cell>
           <cell r="T6">
-            <v>8.7899999999999991</v>
+            <v>46.69</v>
           </cell>
           <cell r="U6">
-            <v>7.6</v>
+            <v>46.69</v>
           </cell>
           <cell r="V6">
-            <v>6.29</v>
+            <v>46.69</v>
           </cell>
           <cell r="W6">
-            <v>6.62</v>
+            <v>46.58</v>
           </cell>
           <cell r="X6">
-            <v>6.53</v>
+            <v>46.56</v>
           </cell>
           <cell r="Y6">
-            <v>7.99</v>
+            <v>46.69</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="8">
         <row r="2">
           <cell r="B2">
-            <v>36.4</v>
-          </cell>
-          <cell r="C2">
-            <v>36.4</v>
-          </cell>
-          <cell r="D2">
-            <v>35.69</v>
-          </cell>
-          <cell r="E2">
-            <v>35.69</v>
-          </cell>
-          <cell r="F2">
-            <v>35.69</v>
-          </cell>
-          <cell r="G2">
-            <v>35.69</v>
-          </cell>
-          <cell r="H2">
-            <v>35.69</v>
-          </cell>
-          <cell r="I2">
-            <v>47.22</v>
-          </cell>
-          <cell r="J2">
-            <v>36.4</v>
-          </cell>
-          <cell r="K2">
-            <v>36.4</v>
-          </cell>
-          <cell r="L2">
-            <v>47.22</v>
-          </cell>
-          <cell r="M2">
-            <v>47.22</v>
-          </cell>
-          <cell r="N2">
-            <v>42</v>
-          </cell>
-          <cell r="O2">
-            <v>38</v>
-          </cell>
-          <cell r="P2">
-            <v>38</v>
-          </cell>
-          <cell r="Q2">
-            <v>47.22</v>
-          </cell>
-          <cell r="R2">
-            <v>47.22</v>
-          </cell>
-          <cell r="S2">
-            <v>47.22</v>
-          </cell>
-          <cell r="T2">
-            <v>47.22</v>
-          </cell>
-          <cell r="U2">
-            <v>47.22</v>
-          </cell>
-          <cell r="V2">
-            <v>47.22</v>
-          </cell>
-          <cell r="W2">
-            <v>47.22</v>
-          </cell>
-          <cell r="X2">
-            <v>47.22</v>
-          </cell>
-          <cell r="Y2">
-            <v>47.22</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>47.22</v>
-          </cell>
-          <cell r="C3">
-            <v>47.22</v>
-          </cell>
-          <cell r="D3">
-            <v>47.22</v>
-          </cell>
-          <cell r="E3">
-            <v>36</v>
-          </cell>
-          <cell r="F3">
-            <v>35.69</v>
-          </cell>
-          <cell r="G3">
-            <v>35.69</v>
-          </cell>
-          <cell r="H3">
-            <v>35.69</v>
-          </cell>
-          <cell r="I3">
-            <v>47.22</v>
-          </cell>
-          <cell r="J3">
-            <v>47.22</v>
-          </cell>
-          <cell r="K3">
-            <v>47.22</v>
-          </cell>
-          <cell r="L3">
-            <v>47.22</v>
-          </cell>
-          <cell r="M3">
-            <v>47.22</v>
-          </cell>
-          <cell r="N3">
-            <v>47.22</v>
-          </cell>
-          <cell r="O3">
-            <v>47.22</v>
-          </cell>
-          <cell r="P3">
-            <v>47.22</v>
-          </cell>
-          <cell r="Q3">
-            <v>47.22</v>
-          </cell>
-          <cell r="R3">
-            <v>47.22</v>
-          </cell>
-          <cell r="S3">
-            <v>47.22</v>
-          </cell>
-          <cell r="T3">
-            <v>47.22</v>
-          </cell>
-          <cell r="U3">
-            <v>47.22</v>
-          </cell>
-          <cell r="V3">
-            <v>47.22</v>
-          </cell>
-          <cell r="W3">
-            <v>47.22</v>
-          </cell>
-          <cell r="X3">
-            <v>36</v>
-          </cell>
-          <cell r="Y3">
-            <v>47.22</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>47.22</v>
-          </cell>
-          <cell r="C4">
-            <v>37.4</v>
-          </cell>
-          <cell r="D4">
-            <v>69.040000000000006</v>
-          </cell>
-          <cell r="E4">
-            <v>37.4</v>
-          </cell>
-          <cell r="F4">
-            <v>35.69</v>
-          </cell>
-          <cell r="G4">
-            <v>37.4</v>
-          </cell>
-          <cell r="H4">
-            <v>37.4</v>
-          </cell>
-          <cell r="I4">
-            <v>37.4</v>
-          </cell>
-          <cell r="J4">
-            <v>37.4</v>
-          </cell>
-          <cell r="K4">
-            <v>38</v>
-          </cell>
-          <cell r="L4">
-            <v>38</v>
-          </cell>
-          <cell r="M4">
-            <v>47.22</v>
-          </cell>
-          <cell r="N4">
-            <v>47.22</v>
-          </cell>
-          <cell r="O4">
-            <v>47.22</v>
-          </cell>
-          <cell r="P4">
-            <v>47.22</v>
-          </cell>
-          <cell r="Q4">
-            <v>47.22</v>
-          </cell>
-          <cell r="R4">
-            <v>47.22</v>
-          </cell>
-          <cell r="S4">
-            <v>47.22</v>
-          </cell>
-          <cell r="T4">
-            <v>47.22</v>
-          </cell>
-          <cell r="U4">
-            <v>47.22</v>
-          </cell>
-          <cell r="V4">
-            <v>47.22</v>
-          </cell>
-          <cell r="W4">
-            <v>95</v>
-          </cell>
-          <cell r="X4">
-            <v>47.22</v>
-          </cell>
-          <cell r="Y4">
-            <v>47.22</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>37</v>
-          </cell>
-          <cell r="C5">
-            <v>35.69</v>
-          </cell>
-          <cell r="D5">
-            <v>35.69</v>
-          </cell>
-          <cell r="E5">
-            <v>35.69</v>
-          </cell>
-          <cell r="F5">
-            <v>35.69</v>
-          </cell>
-          <cell r="G5">
-            <v>35.69</v>
-          </cell>
-          <cell r="H5">
-            <v>47.22</v>
-          </cell>
-          <cell r="I5">
-            <v>47.22</v>
-          </cell>
-          <cell r="J5">
-            <v>47.22</v>
-          </cell>
-          <cell r="K5">
-            <v>47.22</v>
-          </cell>
-          <cell r="L5">
-            <v>36</v>
-          </cell>
-          <cell r="M5">
-            <v>38.4</v>
-          </cell>
-          <cell r="N5">
-            <v>47.22</v>
-          </cell>
-          <cell r="O5">
-            <v>47.22</v>
-          </cell>
-          <cell r="P5">
-            <v>47.22</v>
-          </cell>
-          <cell r="Q5">
-            <v>47.22</v>
-          </cell>
-          <cell r="R5">
-            <v>47.22</v>
-          </cell>
-          <cell r="S5">
-            <v>47.22</v>
-          </cell>
-          <cell r="T5">
-            <v>47.22</v>
-          </cell>
-          <cell r="U5">
-            <v>47.22</v>
-          </cell>
-          <cell r="V5">
-            <v>47.12</v>
-          </cell>
-          <cell r="W5">
-            <v>47.22</v>
-          </cell>
-          <cell r="X5">
-            <v>47.22</v>
-          </cell>
-          <cell r="Y5">
-            <v>47.043333333333329</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>46.66</v>
-          </cell>
-          <cell r="C6">
-            <v>46.69</v>
-          </cell>
-          <cell r="D6">
-            <v>37.4</v>
-          </cell>
-          <cell r="E6">
-            <v>37.4</v>
-          </cell>
-          <cell r="F6">
-            <v>37.4</v>
-          </cell>
-          <cell r="G6">
-            <v>37.4</v>
-          </cell>
-          <cell r="H6">
-            <v>47.22</v>
-          </cell>
-          <cell r="I6">
-            <v>64.64</v>
-          </cell>
-          <cell r="J6">
-            <v>37.4</v>
-          </cell>
-          <cell r="K6">
-            <v>37.4</v>
-          </cell>
-          <cell r="L6">
-            <v>36</v>
-          </cell>
-          <cell r="M6">
-            <v>37.4</v>
-          </cell>
-          <cell r="N6">
-            <v>46.69</v>
-          </cell>
-          <cell r="O6">
-            <v>46.69</v>
-          </cell>
-          <cell r="P6">
-            <v>46.69</v>
-          </cell>
-          <cell r="Q6">
-            <v>46.69</v>
-          </cell>
-          <cell r="R6">
-            <v>46.69</v>
-          </cell>
-          <cell r="S6">
-            <v>46.69</v>
-          </cell>
-          <cell r="T6">
-            <v>46.69</v>
-          </cell>
-          <cell r="U6">
-            <v>46.69</v>
-          </cell>
-          <cell r="V6">
-            <v>46.69</v>
-          </cell>
-          <cell r="W6">
-            <v>46.58</v>
-          </cell>
-          <cell r="X6">
-            <v>46.56</v>
-          </cell>
-          <cell r="Y6">
-            <v>46.69</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="2">
-          <cell r="B2">
             <v>27.98</v>
           </cell>
           <cell r="C2">
@@ -3136,7 +3132,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="10"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4057,7 +4052,7 @@
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5870,11 +5865,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51365E97-6E69-401A-9DFD-893A2C3FF085}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB224AF7-AF06-40B8-9986-34C502BD82F3}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6468,11 +6463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB008B8-ED0A-4A84-975C-A342158CCFB6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB82C02F-BCC0-4FE2-9CCD-B8D1440925A2}">
   <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7091,11 +7086,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A3DC1DB-E732-4F79-89B1-5F652B3EE8D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78952B52-95E9-4A46-956D-99C2442CB011}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7688,11 +7683,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB06EB1E-49A0-417F-AD8B-905096775CB2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC6F8DD-C4F6-4B8F-AEB1-9B49F4112981}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>